<commit_message>
Update Excel files and add TODO file
</commit_message>
<xml_diff>
--- a/pythonSDK/cubagem.xlsx
+++ b/pythonSDK/cubagem.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,14 +463,14 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.42316</v>
+        <v>3.477208</v>
       </c>
       <c r="D2" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -481,14 +481,14 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.379712</v>
+        <v>1.42316</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -499,14 +499,14 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.438598</v>
+        <v>0.379712</v>
       </c>
       <c r="D4" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -517,14 +517,14 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.136128</v>
+        <v>1.438598</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -535,14 +535,14 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.12</v>
+        <v>0.136128</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -553,14 +553,14 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Livros</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3.621928</v>
+        <v>0.12</v>
       </c>
       <c r="D7" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -571,14 +571,14 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Material de Escritório</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>145.403245</v>
+        <v>3.621928</v>
       </c>
       <c r="D8" t="n">
-        <v>267</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
@@ -589,14 +589,14 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>19.836616</v>
+        <v>145.403245</v>
       </c>
       <c r="D9" t="n">
-        <v>46</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10">
@@ -607,32 +607,32 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.245632</v>
+        <v>19.836616</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>A0</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.48</v>
+        <v>0.245632</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -643,14 +643,14 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.354964</v>
+        <v>6.369616</v>
       </c>
       <c r="D12" t="n">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13">
@@ -661,14 +661,14 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.84</v>
+        <v>0.48</v>
       </c>
       <c r="D13" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -679,14 +679,14 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>144.056751</v>
+        <v>0.354964</v>
       </c>
       <c r="D14" t="n">
-        <v>363</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -697,14 +697,14 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Material de Escritório</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1.918676</v>
+        <v>0.84</v>
       </c>
       <c r="D15" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -715,14 +715,14 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Periféricos de Informática</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.12</v>
+        <v>144.019887</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17">
@@ -733,50 +733,50 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.011264</v>
+        <v>1.558676</v>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Periféricos de Informática</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.966</v>
+        <v>0.12</v>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.503072</v>
+        <v>0.011264</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -787,14 +787,14 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.678818</v>
+        <v>5.494232</v>
       </c>
       <c r="D20" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21">
@@ -805,14 +805,14 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Materiais elétricos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.109956</v>
+        <v>0.966</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -823,14 +823,14 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.24</v>
+        <v>1.503072</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -841,14 +841,14 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>130.334596</v>
+        <v>0.678818</v>
       </c>
       <c r="D23" t="n">
-        <v>309</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
@@ -859,14 +859,14 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Materiais elétricos</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.696552</v>
+        <v>0.109956</v>
       </c>
       <c r="D24" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -877,68 +877,68 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Material de Escritório</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.022528</v>
+        <v>0.24</v>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.8</v>
+        <v>130.334596</v>
       </c>
       <c r="D26" t="n">
-        <v>15</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.15312</v>
+        <v>1.696552</v>
       </c>
       <c r="D27" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>125.147933</v>
+        <v>0.022528</v>
       </c>
       <c r="D28" t="n">
-        <v>322</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -949,14 +949,14 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3.015912</v>
+        <v>4.290434</v>
       </c>
       <c r="D29" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30">
@@ -967,14 +967,14 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>Periféricos de Informática</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.424</v>
+        <v>1.8</v>
       </c>
       <c r="D30" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31">
@@ -985,14 +985,14 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Transporte Particular</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.034</v>
+        <v>0.15312</v>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
@@ -1003,209 +1003,209 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.022528</v>
+        <v>125.147933</v>
       </c>
       <c r="D32" t="n">
-        <v>4</v>
+        <v>322</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Maquinário</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.06875000000000001</v>
+        <v>3.015912</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Periféricos de Informática</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2.0615</v>
+        <v>0.424</v>
       </c>
       <c r="D34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Transporte Particular</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.12168</v>
+        <v>0.034</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.09180000000000001</v>
+        <v>0.022528</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Maquinário</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>24.701725</v>
+        <v>0.06875000000000001</v>
       </c>
       <c r="D37" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.6175</v>
+        <v>2.0615</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>B0</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>6.335304</v>
+        <v>0.12168</v>
       </c>
       <c r="D39" t="n">
-        <v>55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>B0</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>5.321979</v>
+        <v>0.222222</v>
       </c>
       <c r="D40" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>B0</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>13.400323</v>
+        <v>0.09180000000000001</v>
       </c>
       <c r="D41" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>B0</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1.43334</v>
+        <v>24.701725</v>
       </c>
       <c r="D42" t="n">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>B0</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.12</v>
+        <v>0.6175</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
@@ -1219,14 +1219,14 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>Maquinário</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>61.753006</v>
+        <v>8.199031</v>
       </c>
       <c r="D44" t="n">
-        <v>104</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45">
@@ -1237,14 +1237,14 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>Maquinário Pesado</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.18412</v>
+        <v>6.335304</v>
       </c>
       <c r="D45" t="n">
-        <v>2</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46">
@@ -1255,14 +1255,14 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>Materiais elétricos</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.312004</v>
+        <v>5.321979</v>
       </c>
       <c r="D46" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47">
@@ -1273,14 +1273,14 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>6.096112</v>
+        <v>13.400323</v>
       </c>
       <c r="D47" t="n">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48">
@@ -1291,14 +1291,14 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>226.549527</v>
+        <v>1.43334</v>
       </c>
       <c r="D48" t="n">
-        <v>525</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49">
@@ -1309,14 +1309,14 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Livros</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>34.881214</v>
+        <v>0.12</v>
       </c>
       <c r="D49" t="n">
-        <v>291</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1327,14 +1327,14 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>Periféricos de Informática</t>
+          <t>Maquinário</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.880007</v>
+        <v>61.753006</v>
       </c>
       <c r="D50" t="n">
-        <v>6</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51">
@@ -1345,14 +1345,14 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>Reagentes</t>
+          <t>Maquinário Pesado</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>7.851938</v>
+        <v>1.18412</v>
       </c>
       <c r="D51" t="n">
-        <v>150</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -1363,14 +1363,14 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>Transporte Particular</t>
+          <t>Materiais elétricos</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2.130475</v>
+        <v>0.312004</v>
       </c>
       <c r="D52" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
@@ -1381,122 +1381,122 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Material de Escritório</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>12.387472</v>
+        <v>6.096112</v>
       </c>
       <c r="D53" t="n">
-        <v>119</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B0</t>
         </is>
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>Ar Condicionado</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1.045264</v>
+        <v>226.549527</v>
       </c>
       <c r="D54" t="n">
-        <v>8</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B0</t>
         </is>
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>7.27204</v>
+        <v>34.881214</v>
       </c>
       <c r="D55" t="n">
-        <v>64</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B0</t>
         </is>
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Periféricos de Informática</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2.917589</v>
+        <v>0.880007</v>
       </c>
       <c r="D56" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B0</t>
         </is>
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Reagentes</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>12.565475</v>
+        <v>7.851938</v>
       </c>
       <c r="D57" t="n">
-        <v>106</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B0</t>
         </is>
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Transporte Particular</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.719516</v>
+        <v>2.130475</v>
       </c>
       <c r="D58" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B0</t>
         </is>
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.445824</v>
+        <v>12.387472</v>
       </c>
       <c r="D59" t="n">
-        <v>12</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60">
@@ -1507,14 +1507,14 @@
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>Maquinário</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>31.564631</v>
+        <v>7.953425</v>
       </c>
       <c r="D60" t="n">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61">
@@ -1525,14 +1525,14 @@
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>Maquinário Pesado</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.28</v>
+        <v>7.27204</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62">
@@ -1543,14 +1543,14 @@
       </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>Maquinário Sensível</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.274304</v>
+        <v>2.917589</v>
       </c>
       <c r="D62" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
@@ -1561,14 +1561,14 @@
       </c>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>Materiais elétricos</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.505848</v>
+        <v>12.685475</v>
       </c>
       <c r="D63" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64">
@@ -1579,14 +1579,14 @@
       </c>
       <c r="B64" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.951259</v>
+        <v>0.719516</v>
       </c>
       <c r="D64" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65">
@@ -1597,14 +1597,14 @@
       </c>
       <c r="B65" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Livros</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>291.367301</v>
+        <v>0.445824</v>
       </c>
       <c r="D65" t="n">
-        <v>624</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66">
@@ -1615,14 +1615,14 @@
       </c>
       <c r="B66" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Maquinário</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>696.948589</v>
+        <v>31.564631</v>
       </c>
       <c r="D66" t="n">
-        <v>183</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67">
@@ -1633,14 +1633,14 @@
       </c>
       <c r="B67" s="1" t="inlineStr">
         <is>
-          <t>Periféricos de Informática</t>
+          <t>Maquinário Pesado</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.032928</v>
+        <v>0.28</v>
       </c>
       <c r="D67" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1651,14 +1651,14 @@
       </c>
       <c r="B68" s="1" t="inlineStr">
         <is>
-          <t>Reagentes</t>
+          <t>Maquinário Sensível</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2.654368</v>
+        <v>0.274304</v>
       </c>
       <c r="D68" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
@@ -1669,14 +1669,14 @@
       </c>
       <c r="B69" s="1" t="inlineStr">
         <is>
-          <t>Transporte Particular</t>
+          <t>Materiais elétricos</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.384</v>
+        <v>0.505848</v>
       </c>
       <c r="D69" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -1687,155 +1687,155 @@
       </c>
       <c r="B70" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Material de Escritório</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2.937472</v>
+        <v>0.951259</v>
       </c>
       <c r="D70" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B71" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.240532</v>
+        <v>294.281461</v>
       </c>
       <c r="D71" t="n">
-        <v>4</v>
+        <v>631</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B72" s="1" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.12075</v>
+        <v>696.948589</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B73" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Periféricos de Informática</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>34.79251</v>
+        <v>1.032928</v>
       </c>
       <c r="D73" t="n">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B74" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Reagentes</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.010125</v>
+        <v>2.654368</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>C0</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B75" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Transporte Particular</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.12</v>
+        <v>0.384</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>C0</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B76" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2.2105</v>
+        <v>2.937472</v>
       </c>
       <c r="D76" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>C0</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="B77" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>5.674772</v>
+        <v>0.240532</v>
       </c>
       <c r="D77" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>C0</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="B78" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.14</v>
+        <v>0.12075</v>
       </c>
       <c r="D78" t="n">
         <v>1</v>
@@ -1844,52 +1844,52 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="B79" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>4.249654</v>
+        <v>34.79251</v>
       </c>
       <c r="D79" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="B80" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>9.447324</v>
+        <v>0.010125</v>
       </c>
       <c r="D80" t="n">
-        <v>195</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C0</t>
         </is>
       </c>
       <c r="B81" s="1" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.06467400000000001</v>
+        <v>0.353256</v>
       </c>
       <c r="D81" t="n">
         <v>2</v>
@@ -1898,12 +1898,12 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C0</t>
         </is>
       </c>
       <c r="B82" s="1" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1916,55 +1916,55 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C0</t>
         </is>
       </c>
       <c r="B83" s="1" t="inlineStr">
         <is>
-          <t>Maquinário</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.25428</v>
+        <v>2.2105</v>
       </c>
       <c r="D83" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C0</t>
         </is>
       </c>
       <c r="B84" s="1" t="inlineStr">
         <is>
-          <t>Materiais elétricos</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.04025</v>
+        <v>5.674772</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C0</t>
         </is>
       </c>
       <c r="B85" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.61368</v>
+        <v>0.14</v>
       </c>
       <c r="D85" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -1975,14 +1975,14 @@
       </c>
       <c r="B86" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>96.039699</v>
+        <v>2.388644</v>
       </c>
       <c r="D86" t="n">
-        <v>187</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87">
@@ -1993,14 +1993,14 @@
       </c>
       <c r="B87" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>3.42465</v>
+        <v>4.249654</v>
       </c>
       <c r="D87" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="88">
@@ -2011,14 +2011,14 @@
       </c>
       <c r="B88" s="1" t="inlineStr">
         <is>
-          <t>Periféricos de Informática</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.978325</v>
+        <v>9.447324</v>
       </c>
       <c r="D88" t="n">
-        <v>17</v>
+        <v>195</v>
       </c>
     </row>
     <row r="89">
@@ -2029,158 +2029,158 @@
       </c>
       <c r="B89" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Ferramentas</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.24</v>
+        <v>0.06467400000000001</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B90" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Livros</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>3.58261</v>
+        <v>0.12</v>
       </c>
       <c r="D90" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B91" s="1" t="inlineStr">
         <is>
-          <t>Eletrodomésticos</t>
+          <t>Maquinário</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.24</v>
+        <v>0.25428</v>
       </c>
       <c r="D91" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B92" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Materiais elétricos</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1.219465</v>
+        <v>0.04025</v>
       </c>
       <c r="D92" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B93" s="1" t="inlineStr">
         <is>
-          <t>Livros</t>
+          <t>Material de Escritório</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.12</v>
+        <v>0.61368</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B94" s="1" t="inlineStr">
         <is>
-          <t>Materiais elétricos</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.13682</v>
+        <v>96.039699</v>
       </c>
       <c r="D94" t="n">
-        <v>3</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B95" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>26.052674</v>
+        <v>3.42465</v>
       </c>
       <c r="D95" t="n">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B96" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Periféricos de Informática</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>85.73945999999999</v>
+        <v>0.978325</v>
       </c>
       <c r="D96" t="n">
-        <v>151</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B97" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1.170992</v>
+        <v>0.24</v>
       </c>
       <c r="D97" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -2191,14 +2191,14 @@
       </c>
       <c r="B98" s="1" t="inlineStr">
         <is>
-          <t>Periféricos de Informática</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.919888</v>
+        <v>2.943576</v>
       </c>
       <c r="D98" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99">
@@ -2209,173 +2209,173 @@
       </c>
       <c r="B99" s="1" t="inlineStr">
         <is>
-          <t>Vidraria</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0.24</v>
+        <v>3.58261</v>
       </c>
       <c r="D99" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B100" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Eletrodomésticos</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4.44</v>
+        <v>0.24</v>
       </c>
       <c r="D100" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B101" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>80.954725</v>
+        <v>1.219465</v>
       </c>
       <c r="D101" t="n">
-        <v>206</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B102" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Livros</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>9.176945</v>
+        <v>0.12</v>
       </c>
       <c r="D102" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B103" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Materiais elétricos</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.120007</v>
+        <v>0.13682</v>
       </c>
       <c r="D103" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B104" s="1" t="inlineStr">
         <is>
-          <t>Transporte Particular</t>
+          <t>Material de Escritório</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0.12</v>
+        <v>26.052674</v>
       </c>
       <c r="D104" t="n">
-        <v>1</v>
+        <v>61</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>C4</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B105" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0.0612</v>
+        <v>85.73945999999999</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>C4</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B106" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.08777699999999999</v>
+        <v>1.170992</v>
       </c>
       <c r="D106" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>C4</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B107" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Periféricos de Informática</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>10.97675</v>
+        <v>0.919888</v>
       </c>
       <c r="D107" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>C4</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B108" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Vidraria</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.216</v>
+        <v>0.24</v>
       </c>
       <c r="D108" t="n">
         <v>1</v>
@@ -2384,142 +2384,142 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="B109" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1.944</v>
+        <v>3.138976</v>
       </c>
       <c r="D109" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="B110" s="1" t="inlineStr">
         <is>
-          <t>Material de Escritório</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1.944</v>
+        <v>4.44</v>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="B111" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Material de Escritório</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1.10153</v>
+        <v>80.954725</v>
       </c>
       <c r="D111" t="n">
-        <v>2</v>
+        <v>206</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="B112" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Mobília</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1.372672</v>
+        <v>9.176945</v>
       </c>
       <c r="D112" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="B113" s="1" t="inlineStr">
         <is>
-          <t>Eletrônicos</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0.03</v>
+        <v>0.120007</v>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="B114" s="1" t="inlineStr">
         <is>
-          <t>Ferramentas</t>
+          <t>Transporte Particular</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="D114" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>C4</t>
         </is>
       </c>
       <c r="B115" s="1" t="inlineStr">
         <is>
-          <t>Mobília</t>
+          <t>Ar Condicionado</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>23.870035</v>
+        <v>0.353256</v>
       </c>
       <c r="D115" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>C4</t>
         </is>
       </c>
       <c r="B116" s="1" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Computadores</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.128</v>
+        <v>0.0612</v>
       </c>
       <c r="D116" t="n">
         <v>1</v>
@@ -2528,36 +2528,288 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>VV</t>
+          <t>C4</t>
         </is>
       </c>
       <c r="B117" s="1" t="inlineStr">
         <is>
-          <t>Computadores</t>
+          <t>Eletrônicos</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6.96</v>
+        <v>0.08777699999999999</v>
       </c>
       <c r="D117" t="n">
-        <v>58</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
+          <t>C4</t>
+        </is>
+      </c>
+      <c r="B118" s="1" t="inlineStr">
+        <is>
+          <t>Mobília</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>10.97675</v>
+      </c>
+      <c r="D118" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>C4</t>
+        </is>
+      </c>
+      <c r="B119" s="1" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>0.216</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B120" s="1" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>1.944</v>
+      </c>
+      <c r="D120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B121" s="1" t="inlineStr">
+        <is>
+          <t>Material de Escritório</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>1.944</v>
+      </c>
+      <c r="D121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B122" s="1" t="inlineStr">
+        <is>
+          <t>Mobília</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>1.10153</v>
+      </c>
+      <c r="D122" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B123" s="1" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>1.372672</v>
+      </c>
+      <c r="D123" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="B124" s="1" t="inlineStr">
+        <is>
+          <t>Ar Condicionado</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>0.12492</v>
+      </c>
+      <c r="D124" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="B125" s="1" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="B126" s="1" t="inlineStr">
+        <is>
+          <t>Ferramentas</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>22.928</v>
+      </c>
+      <c r="D126" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="B127" s="1" t="inlineStr">
+        <is>
+          <t>Materiais elétricos</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="D127" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="B128" s="1" t="inlineStr">
+        <is>
+          <t>Mobília</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>23.870035</v>
+      </c>
+      <c r="D128" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B129" s="1" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="D129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
+        <is>
           <t>VV</t>
         </is>
       </c>
-      <c r="B118" s="1" t="inlineStr">
+      <c r="B130" s="1" t="inlineStr">
+        <is>
+          <t>Ar Condicionado</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>0.54208</v>
+      </c>
+      <c r="D130" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>VV</t>
+        </is>
+      </c>
+      <c r="B131" s="1" t="inlineStr">
+        <is>
+          <t>Computadores</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>6.96</v>
+      </c>
+      <c r="D131" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>VV</t>
+        </is>
+      </c>
+      <c r="B132" s="1" t="inlineStr">
         <is>
           <t>Mobília</t>
         </is>
       </c>
-      <c r="C118" t="n">
+      <c r="C132" t="n">
         <v>36.195091</v>
       </c>
-      <c r="D118" t="n">
+      <c r="D132" t="n">
         <v>115</v>
       </c>
     </row>

</xml_diff>